<commit_message>
update the qa pairs
</commit_message>
<xml_diff>
--- a/qa_annotated.xlsx
+++ b/qa_annotated.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fengluo/Desktop/project/agent_project/qa_benchmark/test_topics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D74E840-10DE-8D48-A284-4C2E3B994129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A9AC4-8719-1E44-8560-A31CC4D459F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{DA7663B6-E541-2A47-9834-E5AC075561A2}"/>
+    <workbookView xWindow="30240" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{DA7663B6-E541-2A47-9834-E5AC075561A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="qa_pair" sheetId="2" r:id="rId1"/>
-    <sheet name="usage" sheetId="4" r:id="rId2"/>
+    <sheet name="qa_pair" sheetId="4" r:id="rId1"/>
+    <sheet name="qa_pair_old" sheetId="2" r:id="rId2"/>
     <sheet name="data_source" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="139">
   <si>
     <t>Paper</t>
   </si>
@@ -332,13 +332,139 @@
   </si>
   <si>
     <t>llm_for_tabular_data_text-to-sql</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Bird dev</t>
+  </si>
+  <si>
+    <t>Execution accuracy</t>
+  </si>
+  <si>
+    <t>chase-sql+Gemini 1.5,chase-sql+Claude3.5 Sonnet</t>
+  </si>
+  <si>
+    <t>deepeye-sql Qwen3-Coder-30B-A3B-Instruct,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct</t>
+  </si>
+  <si>
+    <t>opensearch-sql Gpt-4o,opensearch-sql Gpt-4o+w/o consistency and vote,opensearch-sql Gpt-4</t>
+  </si>
+  <si>
+    <t>Ranking (best-&gt;worst)</t>
+  </si>
+  <si>
+    <t>ominisql ominisql-32b maj,ominisql ominisql-7b-lora maj,ominisql ominisql-7b maj,ominisql ominisql-14b maj,ominisql ominisql-14b-lora maj,ominisql ominisql-32b gre,ominisql ominisql-14b gre,ominisql ominisql-7b gre,ominisql ominisql-14b-lora gre, ominisql ominisql-7b-lora gre</t>
+  </si>
+  <si>
+    <t>distillery ft-gpt-4o,distillery gemini 1.5 pro,distillery llama 3.1-405b</t>
+  </si>
+  <si>
+    <t>share-8b,share-3.8b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,XinYan-sql</t>
+  </si>
+  <si>
+    <t>chase-sql,reasoning-sql,XinYan-sql</t>
+  </si>
+  <si>
+    <t>XinYan-sql,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,chase-sql Claude3.5 Sonnet</t>
+  </si>
+  <si>
+    <t>opensearch-sql,reasoning-sql,share</t>
+  </si>
+  <si>
+    <t>opensearch-sql Gpt-4o,opensearch-sql Gpt-4o+w/o consistency and vote,reasoning-sql Qwen-14B,share-8b,share-3.8b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,share</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,share-8b,share-3.8b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,XinYan-sql,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql,reasoning-sql,share</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet,share-8b,share-3.8b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql,reasoning-sql,XinYan-sql</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,XinYan-sql,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql,XinYan-sql,distillery</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,XinYan-sql,chase-sql Gemini 1.5,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet,distillery ft-gpt-4o,distillery gemini 1.5 pro,distillery llama 3.1-405b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql,reasoning-sql,distillery</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet,distillery ft-gpt-4o,distillery gemini 1.5 pro,distillery llama 3.1-405b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql,reasoning-sql,distillery,share,XinYan-sql</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,XinYan-sql,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet,distillery ft-gpt-4o,share-8b,share-3.8b,distillery gemini 1.5 pro,distillery llama 3.1-405b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql,reasoning-sql,distillery,XinYan-sql,opensearch-sql</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,XinYan-sql,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet,opensearch-sql Gpt-4o,opensearch-sql Gpt-4o+w/o consistency and vote,distillery ft-gpt-4o,distillery gemini 1.5 pro,distillery llama 3.1-405b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql,reasoning-sql,distillery,share,opensearch-sql</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet,opensearch-sql Gpt-4o,opensearch-sql Gpt-4o+w/o consistency and vote,distillery ft-gpt-4o,share-8b,share-3.8b,distillery gemini 1.5 pro,distillery llama 3.1-405b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql,reasoning-sql,distillery,share,opensearch-sql,XinYan-sql</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,XinYan-sql,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet,opensearch-sql Gpt-4o,opensearch-sql Gpt-4o+w/o consistency and vote,distillery ft-gpt-4o,share-8b,share-3.8b,distillery gemini 1.5 pro,distillery llama 3.1-405b</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, deepeye-sql,chase-sql</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,deepeye-sql Qwen3-Coder-30B-A3B-Instruct,chase-sql Gemini 1.5,deepeye-sql Gemma3-27B-Instruct,deepeye-sql Qwen2.5-Coder-32B-Instruct,chase-sql Claude3.5 Sonnet</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql, reasoning-sql,chase-sql</t>
+  </si>
+  <si>
+    <t>Agentar-scale-sql,chase-sql Gemini 1.5,reasoning-sql Qwen-14B,chase-sql Claude3.5 Sonnet</t>
+  </si>
+  <si>
+    <t>Bird test,Bird dev</t>
+  </si>
+  <si>
+    <t>Spider test,Bird dev,Bird test</t>
+  </si>
+  <si>
+    <t>Spider test,Bird dev</t>
+  </si>
+  <si>
+    <t>Spider test,Bird test,Bird dev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,6 +476,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -389,11 +521,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,11 +862,622 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA7D0B1-703E-F74D-9F7A-C91B197C8F95}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="79.1640625" customWidth="1"/>
+    <col min="5" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="255.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA46EEFA-09DC-1A45-9802-6574CA66BE78}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1385,20 +2131,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA7D0B1-703E-F74D-9F7A-C91B197C8F95}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>